<commit_message>
data updated on July 17, 14:54
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A1F3B3-A60B-4FAA-AE36-602B7B01C65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F11BD8F-D9A1-4D51-B439-E4947BEDCE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4074" yWindow="180" windowWidth="17412" windowHeight="12192" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="8622" yWindow="66" windowWidth="17412" windowHeight="12192" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Sat</t>
   </si>
@@ -105,6 +105,14 @@
   </si>
   <si>
     <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cc_1st</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cc_2nd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -240,7 +248,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,6 +296,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA47824-958D-4F3C-882E-E06E483B676D}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -626,21 +637,27 @@
     <col min="6" max="6" width="11.046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" s="18"/>
+      <c r="G1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
@@ -656,7 +673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A3" s="6">
         <v>44747</v>
       </c>
@@ -676,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="6">
         <v>44748</v>
       </c>
@@ -696,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="6">
         <v>44749</v>
       </c>
@@ -716,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="6">
         <v>44750</v>
       </c>
@@ -735,8 +752,14 @@
       <c r="F6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G6" s="12">
+        <v>226</v>
+      </c>
+      <c r="H6" s="12">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="6">
         <v>44751</v>
       </c>
@@ -755,8 +778,9 @@
       <c r="F7" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="6">
         <v>44752</v>
       </c>
@@ -776,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="6">
         <v>44753</v>
       </c>
@@ -795,8 +819,14 @@
       <c r="F9" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G9" s="12">
+        <v>2670</v>
+      </c>
+      <c r="H9" s="12">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="6">
         <v>44754</v>
       </c>
@@ -815,8 +845,14 @@
       <c r="F10" s="5">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G10" s="12">
+        <v>3054</v>
+      </c>
+      <c r="H10">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="6">
         <v>44755</v>
       </c>
@@ -835,8 +871,14 @@
       <c r="F11" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G11" s="12">
+        <v>6542</v>
+      </c>
+      <c r="H11" s="12">
+        <v>5937</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" s="6">
         <v>44756</v>
       </c>
@@ -855,8 +897,14 @@
       <c r="F12" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G12" s="12">
+        <v>8982</v>
+      </c>
+      <c r="H12" s="12">
+        <v>6388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" s="6">
         <v>44757</v>
       </c>
@@ -875,20 +923,40 @@
       <c r="F13" s="5">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G13" s="12">
+        <v>10728</v>
+      </c>
+      <c r="H13" s="12">
+        <v>7023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14" s="6">
         <v>44758</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C14" s="3">
+        <v>53</v>
+      </c>
+      <c r="D14" s="5">
+        <v>68</v>
+      </c>
+      <c r="E14" s="12">
+        <v>47</v>
+      </c>
+      <c r="F14" s="5">
+        <v>57</v>
+      </c>
+      <c r="G14" s="12">
+        <v>11914</v>
+      </c>
+      <c r="H14" s="12">
+        <v>7501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="6">
         <v>44759</v>
       </c>
@@ -899,8 +967,14 @@
       <c r="D15" s="5"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G15" s="12">
+        <v>13708</v>
+      </c>
+      <c r="H15" s="12">
+        <v>8640</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" s="6">
         <v>44760</v>
       </c>
@@ -1083,19 +1157,19 @@
       <c r="B31" s="14"/>
       <c r="C31" s="13">
         <f>SUM(C5:C29)</f>
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="D31" s="15">
         <f>SUM(D5:D29)</f>
-        <v>232</v>
+        <v>300</v>
       </c>
       <c r="E31" s="14">
         <f>SUM(E5:E29)</f>
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="F31" s="15">
         <f>SUM(F5:F29)</f>
-        <v>177</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
data updated on July 18, 09:54
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F11BD8F-D9A1-4D51-B439-E4947BEDCE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FCC62A-FC09-4997-8745-089338ED4A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8622" yWindow="66" windowWidth="17412" windowHeight="12192" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="5436" yWindow="0" windowWidth="17412" windowHeight="12192" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -963,10 +963,18 @@
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="3">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5">
+        <v>130</v>
+      </c>
+      <c r="E15" s="12">
+        <v>20</v>
+      </c>
+      <c r="F15" s="5">
+        <v>121</v>
+      </c>
       <c r="G15" s="12">
         <v>13708</v>
       </c>
@@ -1157,19 +1165,19 @@
       <c r="B31" s="14"/>
       <c r="C31" s="13">
         <f>SUM(C5:C29)</f>
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D31" s="15">
         <f>SUM(D5:D29)</f>
-        <v>300</v>
+        <v>430</v>
       </c>
       <c r="E31" s="14">
         <f>SUM(E5:E29)</f>
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F31" s="15">
         <f>SUM(F5:F29)</f>
-        <v>234</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
data updated on July 19, 11:50
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F62D2E1-70EE-4179-BB30-734FB7F96B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81B4FDE-855D-4B72-A959-E7FFA4B483F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5376" yWindow="5874" windowWidth="17412" windowHeight="12192" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="1080" yWindow="1842" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +60,14 @@
   </si>
   <si>
     <t>cc2nd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lzasytocon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cgasytocon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -195,7 +203,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -245,6 +253,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,20 +572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA47824-958D-4F3C-882E-E06E483B676D}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="10.8984375" customWidth="1"/>
-    <col min="5" max="5" width="11.046875" customWidth="1"/>
+    <col min="3" max="4" width="10.8984375" customWidth="1"/>
+    <col min="6" max="7" width="11.046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -585,19 +596,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="4">
         <v>44749</v>
       </c>
@@ -607,14 +624,20 @@
       <c r="C2" s="3">
         <v>0</v>
       </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" s="4">
         <v>44750</v>
       </c>
@@ -625,19 +648,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
         <v>226</v>
       </c>
-      <c r="G3" s="9">
+      <c r="I3" s="9">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" s="4">
         <v>44751</v>
       </c>
@@ -647,15 +676,21 @@
       <c r="C4" s="3">
         <v>8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>8</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="4">
         <v>44752</v>
       </c>
@@ -666,13 +701,19 @@
         <v>25</v>
       </c>
       <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="4">
         <v>44753</v>
       </c>
@@ -682,20 +723,26 @@
       <c r="C6" s="3">
         <v>17</v>
       </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
         <v>12</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
         <v>2670</v>
       </c>
-      <c r="G6" s="9">
+      <c r="I6" s="9">
         <v>2152</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" s="4">
         <v>44754</v>
       </c>
@@ -705,20 +752,26 @@
       <c r="C7" s="3">
         <v>56</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>45</v>
       </c>
-      <c r="F7" s="9">
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
         <v>3054</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>3054</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="4">
         <v>44755</v>
       </c>
@@ -728,20 +781,26 @@
       <c r="C8" s="3">
         <v>50</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9">
         <v>28</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>36</v>
       </c>
-      <c r="F8" s="9">
+      <c r="G8" s="9">
+        <v>7</v>
+      </c>
+      <c r="H8" s="9">
         <v>6542</v>
       </c>
-      <c r="G8" s="9">
+      <c r="I8" s="9">
         <v>5937</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="4">
         <v>44756</v>
       </c>
@@ -751,20 +810,26 @@
       <c r="C9" s="3">
         <v>17</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
         <v>18</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>13</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9">
         <v>8982</v>
       </c>
-      <c r="G9" s="9">
+      <c r="I9" s="9">
         <v>6388</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="4">
         <v>44757</v>
       </c>
@@ -774,20 +839,26 @@
       <c r="C10" s="3">
         <v>58</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
         <v>24</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>42</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
         <v>10728</v>
       </c>
-      <c r="G10" s="9">
+      <c r="I10" s="9">
         <v>7023</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="4">
         <v>44758</v>
       </c>
@@ -797,20 +868,26 @@
       <c r="C11" s="3">
         <v>68</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
         <v>47</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>57</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
         <v>11914</v>
       </c>
-      <c r="G11" s="9">
+      <c r="I11" s="9">
         <v>7501</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="4">
         <v>44759</v>
       </c>
@@ -820,20 +897,26 @@
       <c r="C12" s="3">
         <v>130</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="2">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9">
         <v>20</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>121</v>
       </c>
-      <c r="F12" s="9">
+      <c r="G12" s="9">
+        <v>4</v>
+      </c>
+      <c r="H12" s="9">
         <v>13708</v>
       </c>
-      <c r="G12" s="9">
+      <c r="I12" s="9">
         <v>8640</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="4">
         <v>44760</v>
       </c>
@@ -843,140 +926,202 @@
       <c r="C13" s="3">
         <v>154</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
         <v>27</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2035</v>
+      </c>
+      <c r="I13" s="9">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A14" s="4">
+        <v>44761</v>
+      </c>
+      <c r="B14" s="1">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3">
+        <v>197</v>
+      </c>
+      <c r="D14" s="2">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3">
+        <v>188</v>
+      </c>
+      <c r="G14" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="12"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="14.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="14.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="14.4" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data updated on July 20, 10:22
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81B4FDE-855D-4B72-A959-E7FFA4B483F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA76E6-9F90-42F6-A049-3B9DEB3A629B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1842" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="1458" yWindow="0" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA47824-958D-4F3C-882E-E06E483B676D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -969,13 +969,27 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="4">
+        <v>44762</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3">
+        <v>191</v>
+      </c>
+      <c r="D15" s="9">
+        <v>24</v>
+      </c>
+      <c r="E15" s="9">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3">
+        <v>184</v>
+      </c>
+      <c r="G15" s="9">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="4"/>

</xml_diff>

<commit_message>
data updated on July 22, 11:05
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA76E6-9F90-42F6-A049-3B9DEB3A629B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E40C6E-6FF2-41FE-A0C9-891C8525A534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1458" yWindow="0" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="2376" yWindow="72" windowWidth="20676" windowHeight="11640" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -992,13 +992,27 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="4">
+        <v>44763</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3">
+        <v>201</v>
+      </c>
+      <c r="D16" s="9">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9">
+        <v>44</v>
+      </c>
+      <c r="F16" s="3">
+        <v>190</v>
+      </c>
+      <c r="G16" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="4"/>

</xml_diff>

<commit_message>
data updated on July 23, 11:23
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E40C6E-6FF2-41FE-A0C9-891C8525A534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5466941C-72C6-488F-A045-365016B20871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2376" yWindow="72" windowWidth="20676" windowHeight="11640" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="1962" yWindow="570" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA47824-958D-4F3C-882E-E06E483B676D}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -967,6 +967,12 @@
       <c r="G14" s="9">
         <v>7</v>
       </c>
+      <c r="H14" s="9">
+        <v>3084</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1553</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="4">
@@ -990,6 +996,12 @@
       <c r="G15" s="9">
         <v>23</v>
       </c>
+      <c r="H15" s="9">
+        <v>1089</v>
+      </c>
+      <c r="I15" s="9">
+        <v>313</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="4">
@@ -1013,15 +1025,35 @@
       <c r="G16" s="9">
         <v>8</v>
       </c>
+      <c r="H16" s="9">
+        <v>2302</v>
+      </c>
+      <c r="I16" s="9">
+        <v>374</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
+      <c r="A17" s="4">
+        <v>44764</v>
+      </c>
+      <c r="B17" s="1">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>164</v>
+      </c>
+      <c r="D17" s="9">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3">
+        <v>149</v>
+      </c>
+      <c r="G17" s="9">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="4"/>

</xml_diff>

<commit_message>
data updated on July 31
</commit_message>
<xml_diff>
--- a/lanzhou_covid-19_202207.xlsx
+++ b/lanzhou_covid-19_202207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5466941C-72C6-488F-A045-365016B20871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DA8C0A-EBF4-4B85-B5D2-7DBDD7068502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1962" yWindow="570" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
+    <workbookView xWindow="2046" yWindow="5196" windowWidth="20676" windowHeight="11652" xr2:uid="{A7B0FD49-9A13-43C5-A306-E7C16726DFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,6 +68,14 @@
   </si>
   <si>
     <t>cgasytocon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lzblndtst</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cgblndtst</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,20 +580,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA47824-958D-4F3C-882E-E06E483B676D}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.25" customWidth="1"/>
-    <col min="3" max="4" width="10.8984375" customWidth="1"/>
-    <col min="6" max="7" width="11.046875" customWidth="1"/>
+    <col min="3" max="5" width="10.8984375" customWidth="1"/>
+    <col min="7" max="9" width="11.046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -599,22 +607,28 @@
         <v>7</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="4">
         <v>44749</v>
       </c>
@@ -627,17 +641,19 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="E2" s="2"/>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" s="4">
         <v>44750</v>
       </c>
@@ -650,23 +666,25 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
       <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9">
         <v>226</v>
       </c>
-      <c r="I3" s="9">
+      <c r="K3" s="9">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" s="4">
         <v>44751</v>
       </c>
@@ -679,18 +697,20 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="2"/>
+      <c r="F4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>8</v>
       </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" s="4">
         <v>44752</v>
       </c>
@@ -703,17 +723,19 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>20</v>
       </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" s="4">
         <v>44753</v>
       </c>
@@ -726,23 +748,25 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <v>12</v>
       </c>
-      <c r="G6" s="9">
-        <v>0</v>
-      </c>
       <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9">
         <v>2670</v>
       </c>
-      <c r="I6" s="9">
+      <c r="K6" s="9">
         <v>2152</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" s="4">
         <v>44754</v>
       </c>
@@ -755,23 +779,25 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="2"/>
+      <c r="F7" s="9">
         <v>4</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>45</v>
       </c>
-      <c r="G7" s="9">
-        <v>0</v>
-      </c>
       <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9">
         <v>3054</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>3054</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" s="4">
         <v>44755</v>
       </c>
@@ -784,23 +810,25 @@
       <c r="D8" s="2">
         <v>11</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="2"/>
+      <c r="F8" s="9">
         <v>28</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>36</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>7</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9">
         <v>6542</v>
       </c>
-      <c r="I8" s="9">
+      <c r="K8" s="9">
         <v>5937</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" s="4">
         <v>44756</v>
       </c>
@@ -813,23 +841,25 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="2"/>
+      <c r="F9" s="9">
         <v>18</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>13</v>
       </c>
-      <c r="G9" s="9">
+      <c r="H9" s="9">
         <v>2</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9">
         <v>8982</v>
       </c>
-      <c r="I9" s="9">
+      <c r="K9" s="9">
         <v>6388</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" s="4">
         <v>44757</v>
       </c>
@@ -842,23 +872,25 @@
       <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="2"/>
+      <c r="F10" s="9">
         <v>24</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>42</v>
       </c>
-      <c r="G10" s="9">
+      <c r="H10" s="9">
         <v>1</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9"/>
+      <c r="J10" s="9">
         <v>10728</v>
       </c>
-      <c r="I10" s="9">
+      <c r="K10" s="9">
         <v>7023</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" s="4">
         <v>44758</v>
       </c>
@@ -871,23 +903,25 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="2"/>
+      <c r="F11" s="9">
         <v>47</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>57</v>
       </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
       <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9">
         <v>11914</v>
       </c>
-      <c r="I11" s="9">
+      <c r="K11" s="9">
         <v>7501</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" s="4">
         <v>44759</v>
       </c>
@@ -900,23 +934,25 @@
       <c r="D12" s="2">
         <v>6</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="2"/>
+      <c r="F12" s="9">
         <v>20</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>121</v>
       </c>
-      <c r="G12" s="9">
+      <c r="H12" s="9">
         <v>4</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9"/>
+      <c r="J12" s="9">
         <v>13708</v>
       </c>
-      <c r="I12" s="9">
+      <c r="K12" s="9">
         <v>8640</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="4">
         <v>44760</v>
       </c>
@@ -929,23 +965,25 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="2"/>
+      <c r="F13" s="9">
         <v>27</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>137</v>
       </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
       <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
         <v>2035</v>
       </c>
-      <c r="I13" s="9">
+      <c r="K13" s="9">
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="4">
         <v>44761</v>
       </c>
@@ -958,23 +996,25 @@
       <c r="D14" s="2">
         <v>7</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="2"/>
+      <c r="F14" s="9">
         <v>29</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>188</v>
       </c>
-      <c r="G14" s="9">
+      <c r="H14" s="9">
         <v>7</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9">
         <v>3084</v>
       </c>
-      <c r="I14" s="9">
+      <c r="K14" s="9">
         <v>1553</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="4">
         <v>44762</v>
       </c>
@@ -987,23 +1027,25 @@
       <c r="D15" s="9">
         <v>24</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9">
         <v>39</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>184</v>
       </c>
-      <c r="G15" s="9">
+      <c r="H15" s="9">
         <v>23</v>
       </c>
-      <c r="H15" s="9">
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
         <v>1089</v>
       </c>
-      <c r="I15" s="9">
+      <c r="K15" s="9">
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" s="4">
         <v>44763</v>
       </c>
@@ -1016,23 +1058,25 @@
       <c r="D16" s="9">
         <v>11</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9">
         <v>44</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>190</v>
       </c>
-      <c r="G16" s="9">
+      <c r="H16" s="9">
         <v>8</v>
       </c>
-      <c r="H16" s="9">
+      <c r="I16" s="9"/>
+      <c r="J16" s="9">
         <v>2302</v>
       </c>
-      <c r="I16" s="9">
+      <c r="K16" s="9">
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" s="4">
         <v>44764</v>
       </c>
@@ -1045,143 +1089,359 @@
       <c r="D17" s="9">
         <v>8</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9">
         <v>31</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>149</v>
       </c>
-      <c r="G17" s="9">
+      <c r="H17" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9">
+        <v>2632</v>
+      </c>
+      <c r="K17" s="9">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A18" s="4">
+        <v>44765</v>
+      </c>
+      <c r="B18" s="1">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3">
+        <v>146</v>
+      </c>
+      <c r="D18" s="9">
+        <v>14</v>
+      </c>
+      <c r="E18" s="9">
+        <v>4</v>
+      </c>
+      <c r="F18" s="9">
+        <v>23</v>
+      </c>
+      <c r="G18" s="3">
+        <v>137</v>
+      </c>
+      <c r="H18" s="9">
+        <v>14</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1656</v>
+      </c>
+      <c r="K18" s="9">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A19" s="4">
+        <v>44766</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3">
+        <v>100</v>
+      </c>
+      <c r="D19" s="9">
+        <v>9</v>
+      </c>
+      <c r="E19" s="9">
+        <v>7</v>
+      </c>
+      <c r="F19" s="9">
+        <v>18</v>
+      </c>
+      <c r="G19" s="3">
+        <v>96</v>
+      </c>
+      <c r="H19" s="9">
+        <v>9</v>
+      </c>
+      <c r="I19" s="9">
+        <v>7</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1342</v>
+      </c>
+      <c r="K19" s="9">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A20" s="4">
+        <v>44767</v>
+      </c>
+      <c r="B20" s="1">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3">
+        <v>79</v>
+      </c>
+      <c r="D20" s="9">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>33</v>
+      </c>
+      <c r="G20" s="3">
+        <v>70</v>
+      </c>
+      <c r="H20" s="9">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2</v>
+      </c>
+      <c r="J20" s="9">
+        <v>1096</v>
+      </c>
+      <c r="K20" s="9">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A21" s="4">
+        <v>44768</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3">
+        <v>75</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2</v>
+      </c>
+      <c r="E21" s="9">
+        <v>3</v>
+      </c>
+      <c r="F21" s="9">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>72</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>3</v>
+      </c>
+      <c r="J21" s="9">
+        <v>982</v>
+      </c>
+      <c r="K21" s="9">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A22" s="4">
+        <v>44769</v>
+      </c>
+      <c r="B22" s="1">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3">
+        <v>41</v>
+      </c>
+      <c r="D22" s="9">
+        <v>11</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3">
+        <v>39</v>
+      </c>
+      <c r="H22" s="9">
+        <v>10</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
+      <c r="J22" s="9">
+        <v>2276</v>
+      </c>
+      <c r="K22" s="9">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A23" s="4">
+        <v>44770</v>
+      </c>
+      <c r="B23" s="1">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3">
+        <v>20</v>
+      </c>
+      <c r="D23" s="9">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3">
+        <v>19</v>
+      </c>
+      <c r="H23" s="9">
+        <v>8</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1425</v>
+      </c>
+      <c r="K23" s="9">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A24" s="4">
+        <v>44771</v>
+      </c>
+      <c r="B24" s="1">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3">
+        <v>19</v>
+      </c>
+      <c r="D24" s="9">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3">
+        <v>18</v>
+      </c>
+      <c r="H24" s="9">
+        <v>9</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A25" s="4">
+        <v>44772</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>10</v>
+      </c>
+      <c r="H25" s="9">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="12"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E29" s="2"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="14.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E30" s="6"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="14.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="14.4" thickTop="1" x14ac:dyDescent="0.5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>